<commit_message>
Adding excelHandling directory and logic to make columns in the escel file for the next quarters and weeks to forecast
</commit_message>
<xml_diff>
--- a/dataset/Hackaton DB Final 04.21 (4).xlsx
+++ b/dataset/Hackaton DB Final 04.21 (4).xlsx
@@ -1754,13 +1754,13 @@
         <v>3354935252.13</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>916289416.3499999</v>
+        <v>3273593400</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>2129234704.355187</v>
+        <v>3273759304.805186</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>1256964727.075411</v>
+        <v>3273837162.720054</v>
       </c>
       <c r="H8" s="4" t="n">
         <v>2046159316.690736</v>
@@ -1769,19 +1769,19 @@
         <v>2203542654.663653</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>1479523540.134121</v>
+        <v>2046149837.078962</v>
       </c>
       <c r="K8" s="4" t="n">
-        <v>1307019834.246524</v>
+        <v>2046156718.431006</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>1149939162.767156</v>
+        <v>2046159693.931045</v>
       </c>
       <c r="M8" s="4" t="n">
         <v>2046164699.896084</v>
       </c>
       <c r="N8" s="4" t="n">
-        <v>1628750623.5</v>
+        <v>2046169125</v>
       </c>
       <c r="O8" s="4" t="n">
         <v>2046166955.830266</v>
@@ -2165,103 +2165,103 @@
         <v>1978711682.85</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>536624401.5999999</v>
+        <v>2893928385.25</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>353027431.6551874</v>
+        <v>3854856015.755187</v>
       </c>
       <c r="G12" s="4" t="n">
-        <v>368128099.3548417</v>
+        <v>5886829119.099483</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>-245814176.2140052</v>
+        <v>5272886843.530636</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>368864309.3945987</v>
+        <v>5887565329.13924</v>
       </c>
       <c r="J12" s="4" t="n">
-        <v>368580775.4913361</v>
+        <v>6453908092.180819</v>
       </c>
       <c r="K12" s="4" t="n">
-        <v>342846281.304709</v>
+        <v>7167310482.178673</v>
       </c>
       <c r="L12" s="4" t="n">
-        <v>308970980.6662872</v>
+        <v>8029655712.70414</v>
       </c>
       <c r="M12" s="4" t="n">
-        <v>-601203031.6505203</v>
+        <v>7119481700.387333</v>
       </c>
       <c r="N12" s="4" t="n">
-        <v>177252124.5571055</v>
+        <v>8315355358.094958</v>
       </c>
       <c r="O12" s="4" t="n">
-        <v>2005693964.442241</v>
+        <v>10143797197.98009</v>
       </c>
       <c r="P12" s="4" t="n">
-        <v>3880075246.687034</v>
+        <v>12018178480.22488</v>
       </c>
       <c r="Q12" s="4" t="n">
-        <v>5805541961.060343</v>
+        <v>13943645194.59819</v>
       </c>
       <c r="R12" s="4" t="n">
-        <v>8907002590.281008</v>
+        <v>17045105823.81886</v>
       </c>
       <c r="S12" s="4" t="n">
-        <v>12088037052.16906</v>
+        <v>20226140285.70691</v>
       </c>
       <c r="T12" s="4" t="n">
-        <v>13331954700.16906</v>
+        <v>21470057933.70691</v>
       </c>
       <c r="U12" s="4" t="n">
-        <v>14179803269.16906</v>
+        <v>22317906502.70691</v>
       </c>
       <c r="V12" s="4" t="n">
-        <v>13833639824.16906</v>
+        <v>21971743057.70691</v>
       </c>
       <c r="W12" s="0" t="n">
-        <v>14179636385.16906</v>
+        <v>22317739618.70691</v>
       </c>
       <c r="X12" s="0" t="n">
-        <v>13667076319.16906</v>
+        <v>21805179552.70691</v>
       </c>
       <c r="Y12" s="0" t="n">
-        <v>16166527150.16906</v>
+        <v>24304630383.70691</v>
       </c>
       <c r="Z12" s="0" t="n">
-        <v>18205079231.16906</v>
+        <v>26343182464.70691</v>
       </c>
       <c r="AA12" s="0" t="n">
-        <v>20426963112.16906</v>
+        <v>28565066345.70691</v>
       </c>
       <c r="AB12" s="0" t="n">
-        <v>20192814423.16906</v>
+        <v>28330917656.70691</v>
       </c>
       <c r="AC12" s="0" t="n">
-        <v>20522829589.16906</v>
+        <v>28660932822.70691</v>
       </c>
       <c r="AD12" s="0" t="n">
-        <v>22753143059.16906</v>
+        <v>30891246292.70691</v>
       </c>
       <c r="AE12" s="0" t="n">
-        <v>23882028401.16906</v>
+        <v>32020131634.70691</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>24035964661.16906</v>
+        <v>32174067894.70691</v>
       </c>
       <c r="AG12" s="0" t="n">
-        <v>25269102731.16906</v>
+        <v>33407205964.70691</v>
       </c>
       <c r="AH12" s="0" t="n">
-        <v>26579107501.16906</v>
+        <v>34717210734.70691</v>
       </c>
       <c r="AI12" s="0" t="n">
-        <v>28221386769.16906</v>
+        <v>36359490002.70691</v>
       </c>
       <c r="AJ12" s="0" t="n">
-        <v>29463914742.16906</v>
+        <v>37602017975.70691</v>
       </c>
       <c r="AK12" s="0" t="n">
-        <v>30610703984.16906</v>
+        <v>38748807217.70691</v>
       </c>
     </row>
     <row r="13" ht="10.5" customHeight="1" s="59">
@@ -2280,43 +2280,43 @@
       </c>
       <c r="D13" s="12" t="n"/>
       <c r="E13" s="12" t="n">
-        <v>139884814.3931541</v>
+        <v>-4049998001.956846</v>
       </c>
       <c r="F13" s="12" t="n">
-        <v>139999981.4699614</v>
+        <v>-2905690044.040411</v>
       </c>
       <c r="G13" s="12" t="n">
-        <v>139973232.0187311</v>
+        <v>-889000073.676734</v>
       </c>
       <c r="H13" s="12" t="n">
-        <v>-4610684124.748766</v>
+        <v>908016894.9958746</v>
       </c>
       <c r="I13" s="12" t="n">
-        <v>133152182.6015007</v>
+        <v>1244767893.018836</v>
       </c>
       <c r="J13" s="12" t="n">
-        <v>139962148.383188</v>
+        <v>2132989790.914745</v>
       </c>
       <c r="K13" s="12" t="n">
-        <v>139776569.505137</v>
+        <v>2871927333.517089</v>
       </c>
       <c r="L13" s="12" t="n">
-        <v>139929049.1730887</v>
+        <v>3768294393.348852</v>
       </c>
       <c r="M13" s="12" t="n">
-        <v>-4839390807.755149</v>
+        <v>2881293924.282703</v>
       </c>
       <c r="N13" s="12" t="n">
-        <v>139903893.1295946</v>
+        <v>4185668876.667447</v>
       </c>
       <c r="O13" s="12" t="n">
-        <v>-2116106065.447186</v>
+        <v>6021997168.090668</v>
       </c>
       <c r="P13" s="12" t="n">
-        <v>-232940930.8397427</v>
+        <v>7905162302.698104</v>
       </c>
       <c r="Q13" s="12" t="n">
-        <v>1692532114.423691</v>
+        <v>9830635347.961536</v>
       </c>
       <c r="R13" s="12" t="n"/>
       <c r="S13" s="12" t="n"/>
@@ -2357,13 +2357,13 @@
         <v>2038937754.98</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>5590446425.865001</v>
+        <v>3324968346.84</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>4012105699</v>
+        <v>2911621667.5</v>
       </c>
       <c r="G14" s="4" t="n">
-        <v>4693399015.71364</v>
+        <v>2754235586.22475</v>
       </c>
       <c r="H14" s="4" t="n">
         <v>3534484566.201103</v>
@@ -2372,19 +2372,19 @@
         <v>738135162.0752832</v>
       </c>
       <c r="J14" s="4" t="n">
-        <v>938256007.8486817</v>
+        <v>393461932.8486817</v>
       </c>
       <c r="K14" s="4" t="n">
-        <v>1104115992</v>
+        <v>393462387.4999999</v>
       </c>
       <c r="L14" s="4" t="n">
-        <v>1255145016.125</v>
+        <v>393462387.4999999</v>
       </c>
       <c r="M14" s="4" t="n">
         <v>393462387.4999999</v>
       </c>
       <c r="N14" s="4" t="n">
-        <v>794794022.75</v>
+        <v>393462387.4999999</v>
       </c>
       <c r="O14" s="4" t="n">
         <v>393462387.4999999</v>
@@ -2768,103 +2768,103 @@
         <v>-2482425490.991282</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>-3359971328.792211</v>
+        <v>-5625449407.817211</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>-5214942541.272617</v>
+        <v>-8580904651.797619</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>-6798124163.404654</v>
+        <v>-12103249703.41854</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>-18318796631.49004</v>
+        <v>-23623922171.50393</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>-23806397006.15393</v>
+        <v>-29111522546.16782</v>
       </c>
       <c r="J18" s="4" t="n">
-        <v>-27986166631.89151</v>
+        <v>-33836086246.9054</v>
       </c>
       <c r="K18" s="4" t="n">
-        <v>-29671259931.98201</v>
+        <v>-36231833151.4959</v>
       </c>
       <c r="L18" s="4" t="n">
-        <v>-30533027327.05266</v>
+        <v>-37955283175.19156</v>
       </c>
       <c r="M18" s="4" t="n">
-        <v>-35079804490.99147</v>
+        <v>-42502060339.13037</v>
       </c>
       <c r="N18" s="4" t="n">
-        <v>-35781938604.50492</v>
+        <v>-43605526087.89382</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>-36865104191.92606</v>
+        <v>-44688691675.31496</v>
       </c>
       <c r="P18" s="4" t="n">
-        <v>-37990079985.66824</v>
+        <v>-45813667469.05714</v>
       </c>
       <c r="Q18" s="4" t="n">
-        <v>-38730439619.52979</v>
+        <v>-46554027102.91869</v>
       </c>
       <c r="R18" s="4" t="n">
-        <v>-36875816915.682</v>
+        <v>-44699404399.0709</v>
       </c>
       <c r="S18" s="4" t="n">
-        <v>-34756881735.99857</v>
+        <v>-42580469219.38747</v>
       </c>
       <c r="T18" s="4" t="n">
-        <v>-41084950313.49857</v>
+        <v>-48908537796.88747</v>
       </c>
       <c r="U18" s="4" t="n">
-        <v>-42326820072.24857</v>
+        <v>-50150407555.63747</v>
       </c>
       <c r="V18" s="4" t="n">
-        <v>-50578134085.74857</v>
+        <v>-58401721569.13747</v>
       </c>
       <c r="W18" s="0" t="n">
-        <v>-63443742051.24857</v>
+        <v>-71267329534.63747</v>
       </c>
       <c r="X18" s="0" t="n">
-        <v>-77687245621.74857</v>
+        <v>-85510833105.13747</v>
       </c>
       <c r="Y18" s="0" t="n">
-        <v>-79623825199.09857</v>
+        <v>-87447412682.48747</v>
       </c>
       <c r="Z18" s="0" t="n">
-        <v>-79788860640.59857</v>
+        <v>-87612448123.98747</v>
       </c>
       <c r="AA18" s="0" t="n">
-        <v>-83371459799.09857</v>
+        <v>-91195047282.48747</v>
       </c>
       <c r="AB18" s="0" t="n">
-        <v>-84706198634.84857</v>
+        <v>-92529786118.23747</v>
       </c>
       <c r="AC18" s="0" t="n">
-        <v>-86364709883.39857</v>
+        <v>-94188297366.78748</v>
       </c>
       <c r="AD18" s="0" t="n">
-        <v>-92339205560.89857</v>
+        <v>-100162793044.2875</v>
       </c>
       <c r="AE18" s="0" t="n">
-        <v>-100545530064.3986</v>
+        <v>-108369117547.7875</v>
       </c>
       <c r="AF18" s="0" t="n">
-        <v>-106564300481.1486</v>
+        <v>-114387887964.5375</v>
       </c>
       <c r="AG18" s="0" t="n">
-        <v>-117272974304.6986</v>
+        <v>-125096561788.0875</v>
       </c>
       <c r="AH18" s="0" t="n">
-        <v>-125649727027.1986</v>
+        <v>-133473314510.5875</v>
       </c>
       <c r="AI18" s="0" t="n">
-        <v>-126632167998.6986</v>
+        <v>-134455755482.0875</v>
       </c>
       <c r="AJ18" s="0" t="n">
-        <v>-127429178293.4486</v>
+        <v>-135252765776.8375</v>
       </c>
       <c r="AK18" s="0" t="n">
-        <v>-130391129751.9986</v>
+        <v>-138214717235.3875</v>
       </c>
     </row>
     <row r="19" ht="10.5" customHeight="1" s="59">
@@ -2883,43 +2883,43 @@
       </c>
       <c r="D19" s="12" t="n"/>
       <c r="E19" s="12" t="n">
-        <v>-15488622758.53059</v>
+        <v>-13223144679.50558</v>
       </c>
       <c r="F19" s="12" t="n">
-        <v>-14494470066.84175</v>
+        <v>-15659464114.36675</v>
       </c>
       <c r="G19" s="12" t="n">
-        <v>-17690437898.26058</v>
+        <v>-19117236579.2967</v>
       </c>
       <c r="H19" s="12" t="n">
-        <v>-26632912871.24008</v>
+        <v>-31938038411.25397</v>
       </c>
       <c r="I19" s="12" t="n">
-        <v>-26233157805.11337</v>
+        <v>-31538283345.12726</v>
       </c>
       <c r="J19" s="12" t="n">
-        <v>-30420520506.00697</v>
+        <v>-35180851971.02086</v>
       </c>
       <c r="K19" s="12" t="n">
-        <v>-32302874398.22114</v>
+        <v>-37442140408.73502</v>
       </c>
       <c r="L19" s="12" t="n">
-        <v>-33372666662.73191</v>
+        <v>-39071557253.62081</v>
       </c>
       <c r="M19" s="12" t="n">
-        <v>-36166114893.24416</v>
+        <v>-43588370741.38306</v>
       </c>
       <c r="N19" s="12" t="n">
-        <v>-37666852244.98915</v>
+        <v>-44687776457.87805</v>
       </c>
       <c r="O19" s="12" t="n">
-        <v>-37955716603.17449</v>
+        <v>-45779304086.56339</v>
       </c>
       <c r="P19" s="12" t="n">
-        <v>-39003769164.94055</v>
+        <v>-46827356648.32944</v>
       </c>
       <c r="Q19" s="12" t="n">
-        <v>-39723462881.3621</v>
+        <v>-47547050364.75099</v>
       </c>
       <c r="R19" s="12" t="n"/>
       <c r="S19" s="12" t="n"/>
@@ -9146,67 +9146,67 @@
         <v>4000</v>
       </c>
       <c r="O5" s="16" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="P5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="Q5" s="4" t="n">
-        <v>1465</v>
+        <v>4000</v>
       </c>
       <c r="R5" s="4" t="n">
-        <v>910</v>
+        <v>4000</v>
       </c>
       <c r="S5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="T5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="U5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="V5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="W5" s="4" t="n">
-        <v>910</v>
+        <v>4000</v>
       </c>
       <c r="X5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="Y5" s="4" t="n">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="Z5" s="4" t="n">
-        <v>2940</v>
+        <v>4000</v>
       </c>
       <c r="AA5" s="4" t="n">
-        <v>2380</v>
+        <v>4000</v>
       </c>
       <c r="AB5" s="4" t="n">
-        <v>3270</v>
+        <v>4000</v>
       </c>
       <c r="AC5" s="4" t="n">
-        <v>2710</v>
+        <v>4000</v>
       </c>
       <c r="AD5" s="4" t="n">
-        <v>2150</v>
+        <v>4000</v>
       </c>
       <c r="AE5" s="4" t="n">
-        <v>1590</v>
+        <v>4000</v>
       </c>
       <c r="AF5" s="4" t="n">
-        <v>1030</v>
+        <v>4000</v>
       </c>
       <c r="AG5" s="4" t="n">
-        <v>470</v>
+        <v>4000</v>
       </c>
       <c r="AH5" s="4" t="n">
-        <v>1575</v>
+        <v>4000</v>
       </c>
       <c r="AI5" s="4" t="n">
-        <v>1025</v>
+        <v>4000</v>
       </c>
       <c r="AJ5" s="4" t="n">
         <v>4000</v>
@@ -9224,43 +9224,43 @@
         <v>4000</v>
       </c>
       <c r="AO5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="AP5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="AQ5" s="4" t="n">
-        <v>1470</v>
+        <v>4000</v>
       </c>
       <c r="AR5" s="4" t="n">
-        <v>910</v>
+        <v>4000</v>
       </c>
       <c r="AS5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="AT5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="AU5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="AV5" s="4" t="n">
-        <v>350</v>
+        <v>4000</v>
       </c>
       <c r="AW5" s="4" t="n">
-        <v>2305</v>
+        <v>4000</v>
       </c>
       <c r="AX5" s="4" t="n">
-        <v>1745</v>
+        <v>4000</v>
       </c>
       <c r="AY5" s="4" t="n">
         <v>4000</v>
       </c>
       <c r="AZ5" s="4" t="n">
-        <v>3995</v>
+        <v>4000</v>
       </c>
       <c r="BA5" s="4" t="n">
-        <v>3440</v>
+        <v>4000</v>
       </c>
       <c r="BB5" s="4" t="n">
         <v>2500</v>
@@ -9347,25 +9347,25 @@
         <v>2500</v>
       </c>
       <c r="CD5" s="4" t="n">
-        <v>1940</v>
+        <v>2500</v>
       </c>
       <c r="CE5" s="4" t="n">
-        <v>2165</v>
+        <v>2500</v>
       </c>
       <c r="CF5" s="4" t="n">
-        <v>1605</v>
+        <v>2500</v>
       </c>
       <c r="CG5" s="4" t="n">
-        <v>1045</v>
+        <v>2500</v>
       </c>
       <c r="CH5" s="4" t="n">
-        <v>485</v>
+        <v>2500</v>
       </c>
       <c r="CI5" s="4" t="n">
-        <v>910</v>
+        <v>2500</v>
       </c>
       <c r="CJ5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="CK5" s="4" t="n">
         <v>2500</v>
@@ -9383,28 +9383,28 @@
         <v>2500</v>
       </c>
       <c r="CP5" s="4" t="n">
-        <v>1395</v>
+        <v>2500</v>
       </c>
       <c r="CQ5" s="4" t="n">
-        <v>845</v>
+        <v>2500</v>
       </c>
       <c r="CR5" s="4" t="n">
-        <v>2030</v>
+        <v>2500</v>
       </c>
       <c r="CS5" s="4" t="n">
-        <v>1470</v>
+        <v>2500</v>
       </c>
       <c r="CT5" s="4" t="n">
-        <v>910</v>
+        <v>2500</v>
       </c>
       <c r="CU5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="CV5" s="4" t="n">
-        <v>910</v>
+        <v>2500</v>
       </c>
       <c r="CW5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="CX5" s="4" t="n">
         <v>2500</v>
@@ -9422,34 +9422,34 @@
         <v>2500</v>
       </c>
       <c r="DC5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="DD5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="DE5" s="4" t="n">
-        <v>2030</v>
+        <v>2500</v>
       </c>
       <c r="DF5" s="4" t="n">
-        <v>1470</v>
+        <v>2500</v>
       </c>
       <c r="DG5" s="4" t="n">
-        <v>910</v>
+        <v>2500</v>
       </c>
       <c r="DH5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="DI5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="DJ5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="DK5" s="4" t="n">
         <v>2500</v>
       </c>
       <c r="DL5" s="4" t="n">
-        <v>2105</v>
+        <v>2500</v>
       </c>
       <c r="DM5" s="4" t="n">
         <v>2500</v>
@@ -9509,19 +9509,19 @@
         <v>2500</v>
       </c>
       <c r="EF5" s="4" t="n">
-        <v>2095</v>
+        <v>2500</v>
       </c>
       <c r="EG5" s="4" t="n">
-        <v>1535</v>
+        <v>2500</v>
       </c>
       <c r="EH5" s="4" t="n">
-        <v>980</v>
+        <v>2500</v>
       </c>
       <c r="EI5" s="4" t="n">
-        <v>910</v>
+        <v>2500</v>
       </c>
       <c r="EJ5" s="4" t="n">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="EK5" s="4" t="n">
         <v>2500</v>
@@ -10467,67 +10467,67 @@
         <v>5437</v>
       </c>
       <c r="O6" s="16" t="n">
-        <v>6450</v>
+        <v>2800</v>
       </c>
       <c r="P6" s="4" t="n">
-        <v>7250</v>
+        <v>3600</v>
       </c>
       <c r="Q6" s="4" t="n">
-        <v>6935</v>
+        <v>4400</v>
       </c>
       <c r="R6" s="4" t="n">
-        <v>7660</v>
+        <v>4570</v>
       </c>
       <c r="S6" s="4" t="n">
-        <v>7368</v>
+        <v>3718</v>
       </c>
       <c r="T6" s="4" t="n">
-        <v>6819</v>
+        <v>3169</v>
       </c>
       <c r="U6" s="4" t="n">
-        <v>8151</v>
+        <v>4501</v>
       </c>
       <c r="V6" s="4" t="n">
-        <v>8350</v>
+        <v>4700</v>
       </c>
       <c r="W6" s="4" t="n">
-        <v>7790</v>
+        <v>4700</v>
       </c>
       <c r="X6" s="4" t="n">
-        <v>8350</v>
+        <v>4700</v>
       </c>
       <c r="Y6" s="4" t="n">
-        <v>5200</v>
+        <v>4700</v>
       </c>
       <c r="Z6" s="4" t="n">
-        <v>5760</v>
+        <v>4700</v>
       </c>
       <c r="AA6" s="4" t="n">
-        <v>6320</v>
+        <v>4700</v>
       </c>
       <c r="AB6" s="4" t="n">
-        <v>4430</v>
+        <v>3700</v>
       </c>
       <c r="AC6" s="4" t="n">
-        <v>4990</v>
+        <v>3700</v>
       </c>
       <c r="AD6" s="4" t="n">
-        <v>5550</v>
+        <v>3700</v>
       </c>
       <c r="AE6" s="4" t="n">
-        <v>6110</v>
+        <v>3700</v>
       </c>
       <c r="AF6" s="4" t="n">
-        <v>6670</v>
+        <v>3700</v>
       </c>
       <c r="AG6" s="4" t="n">
-        <v>7230</v>
+        <v>3700</v>
       </c>
       <c r="AH6" s="4" t="n">
-        <v>6125</v>
+        <v>3700</v>
       </c>
       <c r="AI6" s="4" t="n">
-        <v>6675</v>
+        <v>3700</v>
       </c>
       <c r="AJ6" s="4" t="n">
         <v>3700</v>
@@ -10545,43 +10545,43 @@
         <v>3700</v>
       </c>
       <c r="AO6" s="4" t="n">
-        <v>7150</v>
+        <v>3500</v>
       </c>
       <c r="AP6" s="4" t="n">
-        <v>7150</v>
+        <v>3500</v>
       </c>
       <c r="AQ6" s="4" t="n">
-        <v>6030</v>
+        <v>3500</v>
       </c>
       <c r="AR6" s="4" t="n">
-        <v>6590</v>
+        <v>3500</v>
       </c>
       <c r="AS6" s="4" t="n">
-        <v>7150</v>
+        <v>3500</v>
       </c>
       <c r="AT6" s="4" t="n">
-        <v>7150</v>
+        <v>3500</v>
       </c>
       <c r="AU6" s="4" t="n">
-        <v>7150</v>
+        <v>3500</v>
       </c>
       <c r="AV6" s="4" t="n">
-        <v>7150</v>
+        <v>3500</v>
       </c>
       <c r="AW6" s="4" t="n">
-        <v>5195</v>
+        <v>3500</v>
       </c>
       <c r="AX6" s="4" t="n">
-        <v>5755</v>
+        <v>3500</v>
       </c>
       <c r="AY6" s="4" t="n">
         <v>3500</v>
       </c>
       <c r="AZ6" s="4" t="n">
-        <v>3505</v>
+        <v>3500</v>
       </c>
       <c r="BA6" s="4" t="n">
-        <v>4060</v>
+        <v>3500</v>
       </c>
       <c r="BB6" s="4" t="n">
         <v>5000</v>
@@ -10668,25 +10668,25 @@
         <v>500</v>
       </c>
       <c r="CD6" s="4" t="n">
-        <v>1060</v>
+        <v>500</v>
       </c>
       <c r="CE6" s="4" t="n">
-        <v>835</v>
+        <v>500</v>
       </c>
       <c r="CF6" s="4" t="n">
-        <v>1395</v>
+        <v>500</v>
       </c>
       <c r="CG6" s="4" t="n">
-        <v>1955</v>
+        <v>500</v>
       </c>
       <c r="CH6" s="4" t="n">
-        <v>2515</v>
+        <v>500</v>
       </c>
       <c r="CI6" s="4" t="n">
-        <v>2090</v>
+        <v>500</v>
       </c>
       <c r="CJ6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="CK6" s="4" t="n">
         <v>500</v>
@@ -10704,28 +10704,28 @@
         <v>500</v>
       </c>
       <c r="CP6" s="4" t="n">
-        <v>1605</v>
+        <v>500</v>
       </c>
       <c r="CQ6" s="4" t="n">
-        <v>2155</v>
+        <v>500</v>
       </c>
       <c r="CR6" s="4" t="n">
-        <v>970</v>
+        <v>500</v>
       </c>
       <c r="CS6" s="4" t="n">
-        <v>1530</v>
+        <v>500</v>
       </c>
       <c r="CT6" s="4" t="n">
-        <v>2090</v>
+        <v>500</v>
       </c>
       <c r="CU6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="CV6" s="4" t="n">
-        <v>2090</v>
+        <v>500</v>
       </c>
       <c r="CW6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="CX6" s="4" t="n">
         <v>500</v>
@@ -10743,34 +10743,34 @@
         <v>500</v>
       </c>
       <c r="DC6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="DD6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="DE6" s="4" t="n">
-        <v>970</v>
+        <v>500</v>
       </c>
       <c r="DF6" s="4" t="n">
-        <v>1530</v>
+        <v>500</v>
       </c>
       <c r="DG6" s="4" t="n">
-        <v>2090</v>
+        <v>500</v>
       </c>
       <c r="DH6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="DI6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="DJ6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="DK6" s="4" t="n">
         <v>500</v>
       </c>
       <c r="DL6" s="4" t="n">
-        <v>895</v>
+        <v>500</v>
       </c>
       <c r="DM6" s="4" t="n">
         <v>500</v>
@@ -10830,19 +10830,19 @@
         <v>500</v>
       </c>
       <c r="EF6" s="4" t="n">
-        <v>905</v>
+        <v>500</v>
       </c>
       <c r="EG6" s="4" t="n">
-        <v>1465</v>
+        <v>500</v>
       </c>
       <c r="EH6" s="4" t="n">
-        <v>2020</v>
+        <v>500</v>
       </c>
       <c r="EI6" s="4" t="n">
-        <v>2090</v>
+        <v>500</v>
       </c>
       <c r="EJ6" s="4" t="n">
-        <v>2650</v>
+        <v>500</v>
       </c>
       <c r="EK6" s="4" t="n">
         <v>500</v>

</xml_diff>